<commit_message>
Updated and cleaned list of LSMPAs
</commit_message>
<xml_diff>
--- a/data/list_LSMPAs.xlsx
+++ b/data/list_LSMPAs.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynham/Documents/GitHub/LSMPA_spillover/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A15F4E2-54EA-9A48-8D22-4BA2DB2C52FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB3D2FB-0877-1A4B-BAB0-D13AEB6713F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16920" xr2:uid="{D1B78ED1-9CC7-5D4E-973A-0C3BB5995D36}"/>
+    <workbookView xWindow="2100" yWindow="800" windowWidth="28040" windowHeight="16920" xr2:uid="{D1B78ED1-9CC7-5D4E-973A-0C3BB5995D36}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Wikipedia" sheetId="2" r:id="rId2"/>
+    <sheet name="cleaned" sheetId="3" r:id="rId1"/>
+    <sheet name="draft &amp; notes" sheetId="1" r:id="rId2"/>
+    <sheet name="Wikipedia" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="205">
   <si>
     <t>Name</t>
   </si>
@@ -388,26 +389,302 @@
     <t>Galápagos Marine Reserve</t>
   </si>
   <si>
+    <t>Yes?</t>
+  </si>
+  <si>
     <t>Area (km^2)</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Established in 1998 but apparently not "enforced" until 2003</t>
   </si>
   <si>
     <t>https://www.int-res.com/articles/feature/m585p001.pdf</t>
+  </si>
+  <si>
+    <t>Expanded in 2016</t>
+  </si>
+  <si>
+    <t>Date Created</t>
+  </si>
+  <si>
+    <t>Only within 50 nmi of each island</t>
+  </si>
+  <si>
+    <t>https://sdgs.un.org/partnerships/marae-moana-cook-islands-marine-park-0</t>
+  </si>
+  <si>
+    <t>Marae Moana 1</t>
+  </si>
+  <si>
+    <t>Marae Moana 2</t>
+  </si>
+  <si>
+    <t>https://mer-de-corail.gouv.nc/en/missions-protect/current-regulations</t>
+  </si>
+  <si>
+    <t>New fishing prohibitions introduced in 2018 but a very small area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
+  </si>
+  <si>
+    <t>Expanded in 2014, 5 different areas</t>
+  </si>
+  <si>
+    <t>Pacific Remote Islands 1</t>
+  </si>
+  <si>
+    <t>Coral Sea Marine Park - National Park Zone only</t>
+  </si>
+  <si>
+    <t>https://parksaustralia.gov.au/marine/pub/plans/coral-sea-management-plan-2018.pdf</t>
+  </si>
+  <si>
+    <t>Not contiguous</t>
+  </si>
+  <si>
+    <t>Saint Paul &amp; Amsterdam</t>
+  </si>
+  <si>
+    <t>September 15 2016</t>
+  </si>
+  <si>
+    <t>https://www.pewtrusts.org/en/about/news-room/press-releases-and-statements/2016/09/14/pew-applauds-united-kingdoms-designation-of-pitcairn-islands-marine-reserve</t>
+  </si>
+  <si>
+    <t>https://mpatlas.org/zones/7707499</t>
+  </si>
+  <si>
+    <t>13th November 2020</t>
+  </si>
+  <si>
+    <t>https://tristandc.com/government/news-2020-11-12-mpzgov13nov2020.php</t>
+  </si>
+  <si>
+    <t>Tristan da Cunha Fully Protected Zone</t>
+  </si>
+  <si>
+    <t>January 1st 2020</t>
+  </si>
+  <si>
+    <t>https://www.pewtrusts.org/en/research-and-analysis/articles/2020/01/01/palau-national-marine-sanctuary-goes-into-effect</t>
+  </si>
+  <si>
+    <t>https://impact.economist.com/ocean/biodiversity-ecosystems-and-resources/chiles-marine-protected-areas-a-case-study-in-coastal-governance</t>
+  </si>
+  <si>
+    <t>Juan Fernández archipelago</t>
+  </si>
+  <si>
+    <t>Some sources say area is 740000</t>
+  </si>
+  <si>
+    <t>Notes 2</t>
+  </si>
+  <si>
+    <t>Notes 1</t>
+  </si>
+  <si>
+    <t>Not yet implemented? https://mpatlas.org/zones/68808636</t>
+  </si>
+  <si>
+    <t>https://www.ascension.gov.ac/map-marker/mpa-marine-protected-area</t>
+  </si>
+  <si>
+    <t>Maybe not yet implemented?</t>
+  </si>
+  <si>
+    <t>Reopened?</t>
+  </si>
+  <si>
+    <t>Revillagigedo</t>
+  </si>
+  <si>
+    <t>Motu Motiro Hiva Marine Park</t>
+  </si>
+  <si>
+    <t>Also known as Sala y Gómez</t>
+  </si>
+  <si>
+    <t>https://bigoceanmanagers.org/mmh</t>
+  </si>
+  <si>
+    <t>It's now part of new Rapa Nui MPA</t>
+  </si>
+  <si>
+    <t>https://mpatlas.org/zones/9175</t>
+  </si>
+  <si>
+    <t>https://mpatlas.org/sites/83</t>
+  </si>
+  <si>
+    <t>https://mpatlas.org/sites/84</t>
+  </si>
+  <si>
+    <t>Niue Moana Mahu Marine Protected Area</t>
+  </si>
+  <si>
+    <t>Lots of different smaller areas combined</t>
+  </si>
+  <si>
+    <t>https://mpatlas.org/sites/67</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Cordillera de Coiba Area of Managed Resources</t>
+  </si>
+  <si>
+    <t>Month Enforced</t>
+  </si>
+  <si>
+    <t>https://www.bluenaturealliance.org/cordillera-de-coiba</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>Expanded from 2015 area of 17,224 km^2</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>https://mpatlas.org/zones/68808474</t>
+  </si>
+  <si>
+    <t>No take areas are part of a larger area</t>
+  </si>
+  <si>
+    <t>Freycinet Marine Park</t>
+  </si>
+  <si>
+    <t>No?</t>
+  </si>
+  <si>
+    <t>South-west corner National Park Zone</t>
+  </si>
+  <si>
+    <t>https://mpatlas.org/sites/45</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Freycinet_Commonwealth_Marine_Reserve</t>
+  </si>
+  <si>
+    <t>https://mpatlas.org/zones/68808475</t>
+  </si>
+  <si>
+    <t>WDPA ID</t>
+  </si>
+  <si>
+    <t>Norfolk Island</t>
+  </si>
+  <si>
+    <t>Argo-Rowley Terrace</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Norfolk_Marine_Park</t>
+  </si>
+  <si>
+    <t>Marianas Trench (Islands Unit)</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>Only part is no-take</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Argo-Rowley_Terrace_Marine_Park</t>
+  </si>
+  <si>
+    <t>555556868_A</t>
+  </si>
+  <si>
+    <t>https://storymaps.arcgis.com/stories/8500ba0b1404463f8cb44153c5234691</t>
+  </si>
+  <si>
+    <t>Not enforced?</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Not in a tuna fishing hotspot</t>
+  </si>
+  <si>
+    <t>Defacto long-term MPA since hardly any fishing inside historically? EEZ established in 1997</t>
+  </si>
+  <si>
+    <t>555556875_A</t>
+  </si>
+  <si>
+    <t>2628_B</t>
+  </si>
+  <si>
+    <t>Monumento Natural Das Ilhas de Trindade, Martim Vaz e Do Monte Columbia</t>
+  </si>
+  <si>
+    <t>354083_A</t>
+  </si>
+  <si>
+    <t>Ocean</t>
+  </si>
+  <si>
+    <t>Pacific</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>Atlantic</t>
+  </si>
+  <si>
+    <t>555556901_A</t>
+  </si>
+  <si>
+    <t>Monumento Natural Do Arquipélago De São Pedro E São Paulo</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>WDPA_ID</t>
+  </si>
+  <si>
+    <t>ocean</t>
+  </si>
+  <si>
+    <t>area_km2</t>
+  </si>
+  <si>
+    <t>month_enforced</t>
+  </si>
+  <si>
+    <t>year_enforced</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -448,13 +725,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -470,12 +766,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2503,75 +2813,526 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F322D286-4693-D745-9B6B-629F1E05FF6E}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6871667-2892-3743-8C2F-3470A250D8F5}">
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="A1" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="16">
+        <v>5</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="16">
+        <v>220201</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="18">
+        <v>1508846</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="16">
+        <v>4</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="16">
+        <v>555624172</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" s="18">
+        <v>834334</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="16">
+        <v>555720256</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="18">
+        <v>688628</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="16">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="16">
+        <v>555512151</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" s="18">
+        <v>640000</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="16">
+        <v>7</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="16">
+        <v>555637336</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="18">
+        <v>579368</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="16">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="16">
+        <v>555622118</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7" s="18">
+        <v>475000</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="16">
+        <v>555651558</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="E8" s="18">
+        <v>440000</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="16">
+        <v>2</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="16">
+        <v>309888</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E9" s="18">
+        <v>408250</v>
+      </c>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="16">
+        <v>8</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="16">
+        <v>555624169</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" s="18">
+        <v>300035</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G10" s="16">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="16">
+        <v>9</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="16">
+        <v>555643507</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11" s="18">
+        <v>262000</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E12" s="18">
+        <v>238400</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="16">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="16">
+        <v>555543712</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" s="18">
+        <v>150000</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="16">
+        <v>3</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="16">
+        <v>555629385</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E14" s="18">
+        <v>148644</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="G14" s="16">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="16">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B15" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="B2">
-        <v>142758.68</v>
-      </c>
-      <c r="C2">
+      <c r="C15" s="16">
+        <v>11753</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15" s="18">
+        <v>142759</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16">
         <v>2003</v>
       </c>
-      <c r="D2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1976000</v>
-      </c>
-      <c r="C3">
-        <v>2017</v>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16" s="16">
+        <v>555705568</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E16" s="18">
+        <v>127003</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="G16" s="16">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E17" s="18">
+        <v>124911</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="G17" s="16">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C18" s="16">
+        <v>555705293</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E18" s="18">
+        <v>67821</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18" s="16">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C19" s="16">
+        <v>555635929</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="E19" s="18">
+        <v>67698</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="G19" s="16">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20" s="18">
+        <v>56792</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="18">
+        <v>54841</v>
+      </c>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" s="16">
+        <v>555635928</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="E22" s="18">
+        <v>47200</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="G22" s="16">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23" s="16">
+        <v>400010</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E23" s="18">
+        <v>42624</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" s="16">
+        <v>555556895</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E24" s="18">
+        <v>41661</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="G24" s="16">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E25" s="18">
+        <v>36050</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="G25" s="16">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>
@@ -2580,11 +3341,920 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F322D286-4693-D745-9B6B-629F1E05FF6E}">
+  <dimension ref="A1:M39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>220201</v>
+      </c>
+      <c r="D2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2">
+        <v>1508846</v>
+      </c>
+      <c r="G2" s="13">
+        <v>2016</v>
+      </c>
+      <c r="H2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K2">
+        <v>2006</v>
+      </c>
+      <c r="L2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3">
+        <v>555624172</v>
+      </c>
+      <c r="D3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3">
+        <v>834334</v>
+      </c>
+      <c r="G3" s="13">
+        <v>2016</v>
+      </c>
+      <c r="H3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J3" t="s">
+        <v>156</v>
+      </c>
+      <c r="K3" t="s">
+        <v>128</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="M3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B4" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4">
+        <v>555720256</v>
+      </c>
+      <c r="D4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="3">
+        <v>688628</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="13">
+        <v>2020</v>
+      </c>
+      <c r="H4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I4" t="s">
+        <v>132</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="K4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5">
+        <v>555512151</v>
+      </c>
+      <c r="D5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5">
+        <v>640000</v>
+      </c>
+      <c r="G5" s="13">
+        <v>2010</v>
+      </c>
+      <c r="H5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J5" t="s">
+        <v>110</v>
+      </c>
+      <c r="K5">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6">
+        <v>555637336</v>
+      </c>
+      <c r="D6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6">
+        <v>579368</v>
+      </c>
+      <c r="H6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I6" t="s">
+        <v>136</v>
+      </c>
+      <c r="J6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K6">
+        <v>2017</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="M6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7">
+        <v>555622118</v>
+      </c>
+      <c r="D7" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7" s="8">
+        <v>475000</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="13">
+        <v>2020</v>
+      </c>
+      <c r="H7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I7" t="s">
+        <v>135</v>
+      </c>
+      <c r="J7" t="s">
+        <v>110</v>
+      </c>
+      <c r="K7">
+        <v>2015</v>
+      </c>
+      <c r="L7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>555651558</v>
+      </c>
+      <c r="D8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E8">
+        <v>440000</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K8">
+        <v>2019</v>
+      </c>
+      <c r="L8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9">
+        <v>309888</v>
+      </c>
+      <c r="D9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E9">
+        <v>408250</v>
+      </c>
+      <c r="G9" s="13">
+        <v>2015</v>
+      </c>
+      <c r="H9" t="s">
+        <v>110</v>
+      </c>
+      <c r="J9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K9">
+        <v>2006</v>
+      </c>
+      <c r="L9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10">
+        <v>555624169</v>
+      </c>
+      <c r="D10" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" s="10">
+        <v>300035</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="G10" s="13">
+        <v>2016</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="K10" s="11">
+        <v>42278</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11">
+        <v>555643507</v>
+      </c>
+      <c r="D11" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11" s="3">
+        <v>262000</v>
+      </c>
+      <c r="G11" s="13">
+        <v>2018</v>
+      </c>
+      <c r="I11" t="s">
+        <v>180</v>
+      </c>
+      <c r="L11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E12" s="6">
+        <v>238400</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="13">
+        <v>2018</v>
+      </c>
+      <c r="H12" t="s">
+        <v>110</v>
+      </c>
+      <c r="I12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K12">
+        <v>2018</v>
+      </c>
+      <c r="L12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13">
+        <v>555543712</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" s="3">
+        <v>150000</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="15"/>
+      <c r="I13" t="s">
+        <v>148</v>
+      </c>
+      <c r="K13" s="7">
+        <v>40452</v>
+      </c>
+      <c r="L13" t="s">
+        <v>147</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14">
+        <v>555629385</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E14">
+        <v>148644</v>
+      </c>
+      <c r="F14" t="s">
+        <v>196</v>
+      </c>
+      <c r="G14" s="13">
+        <v>2017</v>
+      </c>
+      <c r="H14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I14" t="s">
+        <v>151</v>
+      </c>
+      <c r="J14" t="s">
+        <v>110</v>
+      </c>
+      <c r="K14" s="7">
+        <v>43009</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15">
+        <v>11753</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15">
+        <v>142759</v>
+      </c>
+      <c r="G15" s="13">
+        <v>2003</v>
+      </c>
+      <c r="H15" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" t="s">
+        <v>112</v>
+      </c>
+      <c r="J15" t="s">
+        <v>110</v>
+      </c>
+      <c r="K15">
+        <v>1998</v>
+      </c>
+      <c r="L15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16">
+        <v>555705568</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E16">
+        <v>127003</v>
+      </c>
+      <c r="F16" t="s">
+        <v>197</v>
+      </c>
+      <c r="G16" s="13">
+        <v>2020</v>
+      </c>
+      <c r="H16" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" t="s">
+        <v>152</v>
+      </c>
+      <c r="J16" t="s">
+        <v>110</v>
+      </c>
+      <c r="K16" s="12">
+        <v>43028</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E17">
+        <v>124911</v>
+      </c>
+      <c r="F17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G17" s="13">
+        <v>2004</v>
+      </c>
+      <c r="H17" t="s">
+        <v>110</v>
+      </c>
+      <c r="I17" t="s">
+        <v>155</v>
+      </c>
+      <c r="J17" t="s">
+        <v>156</v>
+      </c>
+      <c r="L17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>157</v>
+      </c>
+      <c r="C18">
+        <v>555705293</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E18">
+        <v>67821</v>
+      </c>
+      <c r="F18" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18" s="13">
+        <v>2021</v>
+      </c>
+      <c r="I18" t="s">
+        <v>159</v>
+      </c>
+      <c r="L18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>187</v>
+      </c>
+      <c r="C19">
+        <v>555635929</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="E19">
+        <v>67698</v>
+      </c>
+      <c r="F19" t="s">
+        <v>162</v>
+      </c>
+      <c r="G19" s="13">
+        <v>2018</v>
+      </c>
+      <c r="H19" t="s">
+        <v>108</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K19">
+        <v>2018</v>
+      </c>
+      <c r="L19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C20" t="s">
+        <v>188</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20">
+        <v>56792</v>
+      </c>
+      <c r="G20" s="13">
+        <v>2007</v>
+      </c>
+      <c r="H20" t="s">
+        <v>110</v>
+      </c>
+      <c r="I20" t="s">
+        <v>169</v>
+      </c>
+      <c r="J20" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" t="s">
+        <v>193</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21">
+        <v>54841</v>
+      </c>
+      <c r="G21" s="13">
+        <v>2013</v>
+      </c>
+      <c r="H21" t="s">
+        <v>110</v>
+      </c>
+      <c r="I21" t="s">
+        <v>168</v>
+      </c>
+      <c r="J21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22">
+        <v>555635928</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="E22" s="3">
+        <v>47200</v>
+      </c>
+      <c r="F22" t="s">
+        <v>162</v>
+      </c>
+      <c r="G22" s="13">
+        <v>2018</v>
+      </c>
+      <c r="H22" t="s">
+        <v>108</v>
+      </c>
+      <c r="I22" t="s">
+        <v>170</v>
+      </c>
+      <c r="L22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23">
+        <v>400010</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E23" s="3">
+        <v>42624</v>
+      </c>
+      <c r="G23" s="13">
+        <v>2009</v>
+      </c>
+      <c r="H23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24">
+        <v>555556895</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E24" s="3">
+        <v>41661</v>
+      </c>
+      <c r="F24" t="s">
+        <v>176</v>
+      </c>
+      <c r="G24" s="13">
+        <v>2018</v>
+      </c>
+      <c r="H24" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24" t="s">
+        <v>174</v>
+      </c>
+      <c r="L24" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>173</v>
+      </c>
+      <c r="C25" t="s">
+        <v>179</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E25" s="3">
+        <v>36050</v>
+      </c>
+      <c r="F25" t="s">
+        <v>176</v>
+      </c>
+      <c r="G25" s="13">
+        <v>2018</v>
+      </c>
+      <c r="I25" t="s">
+        <v>178</v>
+      </c>
+      <c r="L25" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="13">
+        <v>2017</v>
+      </c>
+      <c r="H33" t="s">
+        <v>115</v>
+      </c>
+      <c r="I33" t="s">
+        <v>116</v>
+      </c>
+      <c r="J33" t="s">
+        <v>110</v>
+      </c>
+      <c r="K33" s="5">
+        <v>42929</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>118</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="13">
+        <v>2017</v>
+      </c>
+      <c r="H34" t="s">
+        <v>115</v>
+      </c>
+      <c r="I34" t="s">
+        <v>116</v>
+      </c>
+      <c r="J34" t="s">
+        <v>110</v>
+      </c>
+      <c r="K34" s="5">
+        <v>42929</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35">
+        <v>1292967</v>
+      </c>
+      <c r="G35" s="13">
+        <v>2014</v>
+      </c>
+      <c r="H35" t="s">
+        <v>121</v>
+      </c>
+      <c r="I35" t="s">
+        <v>119</v>
+      </c>
+      <c r="J35" t="s">
+        <v>110</v>
+      </c>
+      <c r="K35" s="7">
+        <v>41730</v>
+      </c>
+      <c r="L35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>123</v>
+      </c>
+      <c r="G37" s="13">
+        <v>2014</v>
+      </c>
+      <c r="H37" t="s">
+        <v>110</v>
+      </c>
+      <c r="K37">
+        <v>2009</v>
+      </c>
+      <c r="L37" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39">
+        <v>1600000</v>
+      </c>
+      <c r="I39">
+        <v>2016</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M25">
+    <sortCondition descending="1" ref="E2:E25"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="I19" r:id="rId1" xr:uid="{626AC8EA-0113-7D48-A5CF-FF226F65F049}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603A2D2E-B17E-B344-8A3C-E54ADB2141F6}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F3" sqref="B3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>